<commit_message>
[Fucntion] New UI Imported- Frank
</commit_message>
<xml_diff>
--- a/ExcelData/Dialogue.xlsx
+++ b/ExcelData/Dialogue.xlsx
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>WhiteScreenBehavior</t>
   </si>
 </sst>
 </file>
@@ -658,7 +661,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +669,7 @@
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" customWidth="1"/>
+    <col min="4" max="4" width="93.140625" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -784,7 +787,7 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1100,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
[Function] Second Scene First Version- Frank
</commit_message>
<xml_diff>
--- a/ExcelData/Dialogue.xlsx
+++ b/ExcelData/Dialogue.xlsx
@@ -44,8 +44,12 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
+You 0
 PROFESSOR N 1
-T.O.G.A 2</t>
+T.O.G.A 2
+TYRA 3
+ATLAS 4
+Aac 5</t>
         </r>
       </text>
     </comment>
@@ -63,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +89,32 @@
           <t xml:space="preserve">
 1 ShowOptions
 2 Show Questions
-3 Show Effect</t>
+3 Show Effect
+4 Next Scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+if next Operation is 3 then option1 is the id for whitescreen behavior</t>
         </r>
       </text>
     </comment>
@@ -94,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="102">
   <si>
     <t>ID</t>
   </si>
@@ -204,9 +233,6 @@
     <t>Lastly, in front of you are three Biocrystals. They are what gives Biobots life. Choose whichever one you like to form the heart of your Biobot.</t>
   </si>
   <si>
-    <t xml:space="preserve"> I choose the Blue Biocrystal! </t>
-  </si>
-  <si>
     <t xml:space="preserve">I choose the Purple Biocrystal! </t>
   </si>
   <si>
@@ -235,14 +261,236 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>WhiteScreenBehavior</t>
+    <t xml:space="preserve">I choose the Blue Biocrystal! </t>
+  </si>
+  <si>
+    <t>NextEffectID</t>
+  </si>
+  <si>
+    <t>Hey!! Don’t I know you? Yeah it IS you!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait a minute, your voice is kind of familiar. Have we played a game online or something? Wait.. PRINCESSPEACH217!!?  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeah, you look kind of familiar. Didn’t we go to the same school on Earth? You’re the leader of the soccer team right? </t>
+  </si>
+  <si>
+    <t>Yeah, I think I’ve seen you before. Don’t we live on the same street on Earth? You’re the one with that big dog that always barks when I walk past. You’re the girl who owns all those dogs right? What do you have, like, 6 now?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That’s right!! I’m Tyra. I can’t believe we BOTH got recruited! It’s nice to see a familiar face! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OH NO YOU DIDN’T!!!! </t>
+  </si>
+  <si>
+    <t>Angry</t>
+  </si>
+  <si>
+    <t>OH NO I DID!!! What have I done!!?</t>
+  </si>
+  <si>
+    <t>YOU’VE TOTALLY RUINED MY OUTFIT!!!</t>
+  </si>
+  <si>
+    <t>S-sorry! I just -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hey! What’s going on? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SORRY!? You did that on purpose! </t>
+  </si>
+  <si>
+    <t>This kid just barged into me and my Biobot!</t>
+  </si>
+  <si>
+    <t>....Is that all?</t>
+  </si>
+  <si>
+    <t>Puzzle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANNNND he dumped his stinky sticky space juice all over my new outfit! It’s in my hair too!! GROSS!!! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok yikes! Wait. What? Wait a minute.. </t>
+  </si>
+  <si>
+    <t>Thinking</t>
+  </si>
+  <si>
+    <t>What!?</t>
+  </si>
+  <si>
+    <t> Is it really called “Space Juice” oh yeah it is. Wow... so... creative…</t>
+  </si>
+  <si>
+    <t>Unamused</t>
+  </si>
+  <si>
+    <t>Forget about what it’s called! It’s ALL OVER ME!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oh no! I’m so sorry! I was just trying to find my class and I’m completely lost! </t>
+  </si>
+  <si>
+    <t>Grimace</t>
+  </si>
+  <si>
+    <t>Easy to be lost if you’re not watching where you’re going! Besides, your map is upside down, genius.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I think... What Atlas is </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>trying</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to say is “it’s not safe to walk around this busy courtyard with your head in a map.”</t>
+    </r>
+  </si>
+  <si>
+    <t>Don’t worry, errr. What’s your name?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It’s Zac. </t>
+  </si>
+  <si>
+    <t>Right, don’t worry Zac. Atlas is just mad cos you melted his hair wax.</t>
+  </si>
+  <si>
+    <t>Laugh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wow. Okay. I thought we were friends Ty! Why are you on this guy’s side??! Plus.. it’s not wax…. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It's Styling Gel. </t>
+  </si>
+  <si>
+    <t>Uhuh… sure. Well you’ve got ‘styling gel’ running down your face, tough guy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t worry! I got your back Atlas! Zac better watch where he’s going next time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you, new kid! See!? Now there’s the support I needed from you, Ty! </t>
+  </si>
+  <si>
+    <t>Jeez. Always so dramatic..</t>
+  </si>
+  <si>
+    <t>Eyeroll</t>
+  </si>
+  <si>
+    <t>Okay, okay, sorry! I’ll be more careful next time…</t>
+  </si>
+  <si>
+    <t>Sad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great! We better get to class now! We’re all super late! </t>
+  </si>
+  <si>
+    <t>Hey! What about the space juice!?? I’m still completely soaked!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You’re right… We better run fast so you can dry out on the way. Hahaha! </t>
+  </si>
+  <si>
+    <t>NOT FUNNY!!!</t>
+  </si>
+  <si>
+    <t>I think Zac just needs some help. We’re all new here!</t>
+  </si>
+  <si>
+    <t>(to Zac) Hey, it’s alright, Atlas can see that you’re very sorry…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What?! </t>
+  </si>
+  <si>
+    <t>(to Atlas) Hey it was just an accident, why don’t we calm down. I’ll help you out with those stains.... I packed an extra shirt. You can wear it if you want.</t>
+  </si>
+  <si>
+    <t>Ugh… I guess that would work for now…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks……... sorry about that! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you sorry though? </t>
+  </si>
+  <si>
+    <t>YES!!! Of course I am!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’m just messin with you! </t>
+  </si>
+  <si>
+    <t>WE KNOW!!</t>
+  </si>
+  <si>
+    <t>I think Tyra’s right. </t>
+  </si>
+  <si>
+    <r>
+      <t>Right!? Great minds think alike!</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>You need to calm down, Atlas. Zac said sorry like a million times.</t>
+  </si>
+  <si>
+    <t>Sor...</t>
+  </si>
+  <si>
+    <t>Well can your great minds figure out how to remove space juice stains from my uniform before we’re all late to class?</t>
+  </si>
+  <si>
+    <t>You’re right… We better run fast so you can dry out on the way. Hahaha!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT FUNNY!!! </t>
+  </si>
+  <si>
+    <t>IsBigUI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +530,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -303,13 +558,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,10 +916,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,19 +928,20 @@
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="116" customWidth="1"/>
+    <col min="5" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,31 +958,37 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -739,32 +1005,38 @@
         <v>6</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <f>A3</f>
         <v>2</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>38</v>
+      <c r="H2">
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -784,28 +1056,34 @@
         <v>0</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
-        <v>39</v>
-      </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -816,38 +1094,44 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4" si="0">A5</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4" si="0">A5</f>
         <v>4</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
+      <c r="H4">
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -867,31 +1151,37 @@
         <v>0</v>
       </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="2">
         <f>A6</f>
         <v>5</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="3">
+      <c r="M5" s="3">
         <f>A7</f>
         <v>6</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <f>A9</f>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -908,32 +1198,38 @@
         <v>6</v>
       </c>
       <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <f>A8</f>
         <v>7</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
+      <c r="H6">
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -950,32 +1246,38 @@
         <v>6</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <f>A8</f>
         <v>7</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
+      <c r="H7">
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -995,31 +1297,37 @@
         <v>0</v>
       </c>
       <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
         <v>21</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <f>A9</f>
         <v>8</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>22</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <f>A6</f>
         <v>5</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>23</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <f>A7</f>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1030,38 +1338,44 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <f>A10</f>
         <v>9</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
+      <c r="H9">
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1072,38 +1386,44 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <f>A11</f>
         <v>10</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>38</v>
+      <c r="H10">
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1114,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -1123,28 +1443,34 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1161,32 +1487,38 @@
         <v>6</v>
       </c>
       <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <f>A13</f>
         <v>12</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>38</v>
+      <c r="H12">
+        <v>0</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1206,28 +1538,34 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>2</v>
-      </c>
-      <c r="H13" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1247,31 +1585,37 @@
         <v>0</v>
       </c>
       <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>1</v>
       </c>
-      <c r="H14" t="s">
-        <v>29</v>
-      </c>
       <c r="I14">
-        <f>A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="K14">
         <f>A15</f>
         <v>14</v>
       </c>
       <c r="L14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M14">
         <f>A15</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14">
+        <f>A15</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1282,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -1291,28 +1635,35 @@
         <v>0</v>
       </c>
       <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>3</v>
       </c>
-      <c r="H15" t="s">
-        <v>38</v>
-      </c>
       <c r="I15">
-        <v>0</v>
+        <f>I3+1</f>
+        <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>37</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1323,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -1332,24 +1683,2477 @@
         <v>0</v>
       </c>
       <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>3</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16">
+        <f>I15+1</f>
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17">
+        <f>A18</f>
+        <v>17</v>
+      </c>
+      <c r="L17" t="s">
+        <v>42</v>
+      </c>
+      <c r="M17">
+        <f>A18</f>
+        <v>17</v>
+      </c>
+      <c r="N17" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17">
+        <f>A18</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <f>I16+1</f>
+        <v>4</v>
+      </c>
+      <c r="J18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>A20</f>
+        <v>19</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G28" si="1">A21</f>
+        <v>20</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20" t="s">
+        <v>37</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>37</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>37</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22" t="s">
+        <v>37</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>37</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24" t="s">
+        <v>37</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>37</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>37</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>37</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>37</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>37</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>37</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:G34" si="2">A30</f>
+        <v>29</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
+        <v>37</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>37</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
+        <v>37</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>37</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31" t="s">
+        <v>37</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31" t="s">
+        <v>37</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
+        <v>37</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32" t="s">
+        <v>37</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33" t="s">
+        <v>37</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33" t="s">
+        <v>37</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34" t="s">
+        <v>37</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34" t="s">
+        <v>37</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ref="G35:G37" si="3">A36</f>
+        <v>35</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35" t="s">
+        <v>37</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36" t="s">
+        <v>37</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36" t="s">
+        <v>37</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" t="s">
+        <v>69</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>37</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37" t="s">
+        <v>37</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37" t="s">
+        <v>37</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38" si="4">A39</f>
         <v>38</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38" t="s">
+        <v>37</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38" t="s">
+        <v>37</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38" t="s">
+        <v>37</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
-        <v>38</v>
-      </c>
-      <c r="M16">
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f t="shared" ref="G39:G43" si="5">A40</f>
+        <v>39</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>37</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39" t="s">
+        <v>37</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>37</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>37</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40" t="s">
+        <v>37</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40" t="s">
+        <v>37</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>37</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41" t="s">
+        <v>37</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41" t="s">
+        <v>37</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>37</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42" t="s">
+        <v>37</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42" t="s">
+        <v>37</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="5"/>
+        <v>43</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43" t="s">
+        <v>37</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43" t="s">
+        <v>37</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" t="s">
+        <v>78</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ref="G44:G46" si="6">A45</f>
+        <v>44</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44" t="s">
+        <v>37</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44" t="s">
+        <v>37</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44" t="s">
+        <v>37</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45" t="s">
+        <v>37</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45" t="s">
+        <v>37</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="6"/>
+        <v>46</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46" t="s">
+        <v>37</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46" t="s">
+        <v>37</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46" t="s">
+        <v>37</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ref="G47" si="7">A48</f>
+        <v>47</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47" t="s">
+        <v>37</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47" t="s">
+        <v>37</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" t="s">
+        <v>69</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <f t="shared" ref="G48:G58" si="8">A49</f>
+        <v>48</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>37</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48" t="s">
+        <v>37</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48" t="s">
+        <v>37</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>37</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49" t="s">
+        <v>37</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49" t="s">
+        <v>37</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50" t="s">
+        <v>37</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50" t="s">
+        <v>37</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50" t="s">
+        <v>37</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="8"/>
+        <v>51</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>37</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51" t="s">
+        <v>37</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51" t="s">
+        <v>37</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="8"/>
+        <v>52</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>37</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52" t="s">
+        <v>37</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52" t="s">
+        <v>37</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="8"/>
+        <v>53</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>37</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53" t="s">
+        <v>37</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53" t="s">
+        <v>37</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" t="s">
+        <v>76</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="8"/>
+        <v>54</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>37</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54" t="s">
+        <v>37</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54" t="s">
+        <v>37</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" t="s">
+        <v>63</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="8"/>
+        <v>55</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>37</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55" t="s">
+        <v>37</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55" t="s">
+        <v>37</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56" t="s">
+        <v>57</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="8"/>
+        <v>56</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>37</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56" t="s">
+        <v>37</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56" t="s">
+        <v>37</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="8"/>
+        <v>57</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57" t="s">
+        <v>37</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57" t="s">
+        <v>37</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E58" t="s">
+        <v>69</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="8"/>
+        <v>58</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>37</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58" t="s">
+        <v>37</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58" t="s">
+        <v>37</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" t="s">
+        <v>46</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>4</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>37</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59" t="s">
+        <v>37</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59" t="s">
+        <v>37</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <f t="shared" ref="G60:G66" si="9">A61</f>
+        <v>60</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>37</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60" t="s">
+        <v>37</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60" t="s">
+        <v>37</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="9"/>
+        <v>61</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61" t="s">
+        <v>37</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61" t="s">
+        <v>37</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61" t="s">
+        <v>37</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E62" t="s">
+        <v>76</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="9"/>
+        <v>62</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62" t="s">
+        <v>37</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62" t="s">
+        <v>37</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62" t="s">
+        <v>37</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E63" t="s">
+        <v>78</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="9"/>
+        <v>63</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63" t="s">
+        <v>37</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63" t="s">
+        <v>37</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63" t="s">
+        <v>37</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E64" t="s">
+        <v>46</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="9"/>
+        <v>64</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>37</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64" t="s">
+        <v>37</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64" t="s">
+        <v>37</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E65" t="s">
+        <v>76</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="9"/>
+        <v>65</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65" t="s">
+        <v>37</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65" t="s">
+        <v>37</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65" t="s">
+        <v>37</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E66" t="s">
+        <v>69</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="9"/>
+        <v>66</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66" t="s">
+        <v>37</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66" t="s">
+        <v>37</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66" t="s">
+        <v>37</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E67" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>4</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67" t="s">
+        <v>37</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67" t="s">
+        <v>37</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67" t="s">
+        <v>37</v>
+      </c>
+      <c r="O67">
         <v>0</v>
       </c>
     </row>

</xml_diff>